<commit_message>
Lighting - Fixed some issues with the flowfield and lighting, no half way through implementing a compute shader.
</commit_message>
<xml_diff>
--- a/Documentation/WeeklyLog.xlsx
+++ b/Documentation/WeeklyLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\CTP\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D772439C-FBE6-4221-8A15-79AC99F92B5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A3713B-2A26-43C8-BDA4-D9262D05FD78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>C++ Particle System Library</t>
   </si>
@@ -149,6 +149,39 @@
   </si>
   <si>
     <t>Look into signed distance fields for making the particles attracted to an .obj file loaded and then follow the surface of the object.</t>
+  </si>
+  <si>
+    <t>Look into signed distance field and get the particles following the shape of a model.</t>
+  </si>
+  <si>
+    <t>Got the triangles using the signed distance field to compare triangles in a model and find the closest one, then move towards the center point of the nearest triangle. Also refactored code to make it more useable.</t>
+  </si>
+  <si>
+    <t>Get it working on the GPU, on the shader. Look into the LGH and how it will be implemented.</t>
+  </si>
+  <si>
+    <t>Got lighting implemented on the CPU side with it being threaded in order to make it run fast enough.</t>
+  </si>
+  <si>
+    <t>Got a basic LGH working with it apporximating the lights, although still is a bit dodgy when the particles are up close to the model.</t>
+  </si>
+  <si>
+    <t>Look more into the LGH and how to implement better as well as getting the lighting on the GPU.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get lighting on the GPU, look into LGH and how to implement it.  </t>
+  </si>
+  <si>
+    <t>Get lighting implemented into the project with it lighting up a model on the GPU.</t>
+  </si>
+  <si>
+    <t>Get lighting implemented on the GPU with it lighting up the model.</t>
+  </si>
+  <si>
+    <t>Get lighting on the GPU working as well as looking into the LGH more.</t>
+  </si>
+  <si>
+    <t>Got lighting working on the GPU.</t>
   </si>
 </sst>
 </file>
@@ -336,41 +369,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,32 +685,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="14" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="12" customWidth="1"/>
     <col min="2" max="2" width="38.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="50.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="48.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15">
+      <c r="A1" s="13">
         <v>17019105</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -691,7 +724,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="A3" s="14">
         <v>43753</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -705,13 +738,13 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
+      <c r="A4" s="15">
         <v>43760</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="6" t="s">
@@ -719,10 +752,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="A5" s="15">
         <v>43767</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -733,10 +766,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="15">
         <v>43774</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -747,10 +780,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="15">
         <v>43781</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -759,10 +792,10 @@
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
+      <c r="A8" s="15">
         <v>43788</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -773,10 +806,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+      <c r="A9" s="15">
         <v>43795</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -787,10 +820,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+      <c r="A10" s="15">
         <v>43802</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -801,10 +834,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+      <c r="A11" s="15">
         <v>43836</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -815,16 +848,16 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="17">
         <v>43842</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="19" t="s">
         <v>21</v>
       </c>
     </row>
@@ -884,215 +917,224 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="6"/>
+    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>43891</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>43898</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>43905</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>43920</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="A21" s="16"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+      <c r="A22" s="16"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
+      <c r="A23" s="16"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
+      <c r="A24" s="16"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
+      <c r="A25" s="16"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+      <c r="A26" s="16"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
+      <c r="A27" s="16"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+      <c r="A28" s="16"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
+      <c r="A29" s="16"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
+      <c r="A30" s="16"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
+      <c r="A31" s="16"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
+      <c r="A32" s="16"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
+      <c r="A33" s="16"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
+      <c r="A34" s="16"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
+      <c r="A35" s="16"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
+      <c r="A36" s="16"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
+      <c r="A37" s="16"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
+      <c r="A38" s="16"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
+      <c r="A39" s="16"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
+      <c r="A40" s="16"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
+      <c r="A41" s="16"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
+      <c r="A42" s="16"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
+      <c r="A43" s="16"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
+      <c r="A44" s="16"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
+      <c r="A45" s="16"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
+      <c r="A46" s="16"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="18"/>
+      <c r="A47" s="16"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
+      <c r="A48" s="16"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
+      <c r="A49" s="16"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
+      <c r="A50" s="16"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
+      <c r="A51" s="16"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="18"/>
+      <c r="A52" s="16"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
+      <c r="A53" s="16"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="18"/>
+      <c r="A54" s="16"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
+      <c r="A55" s="16"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
+      <c r="A56" s="16"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18"/>
+      <c r="A57" s="16"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="18"/>
+      <c r="A58" s="16"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="18"/>
+      <c r="A59" s="16"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="18"/>
+      <c r="A60" s="16"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="18"/>
+      <c r="A61" s="16"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="18"/>
+      <c r="A62" s="16"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="18"/>
+      <c r="A63" s="16"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="18"/>
+      <c r="A64" s="16"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="18"/>
+      <c r="A65" s="16"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
+      <c r="A66" s="16"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="18"/>
+      <c r="A67" s="16"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="18"/>
+      <c r="A68" s="16"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
+      <c r="A69" s="16"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="18"/>
+      <c r="A70" s="16"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="18"/>
+      <c r="A71" s="16"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="18"/>
+      <c r="A72" s="16"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="18"/>
+      <c r="A73" s="16"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="18"/>
+      <c r="A74" s="16"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="18"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="18"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="18"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="18"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="18"/>
+      <c r="A75" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Flow field - (BROKEN) Tried to implement compute shader but not working
</commit_message>
<xml_diff>
--- a/Documentation/WeeklyLog.xlsx
+++ b/Documentation/WeeklyLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\CTP\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A3713B-2A26-43C8-BDA4-D9262D05FD78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A90F98-5FAB-4685-AB7D-F062C86BDABF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>C++ Particle System Library</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Get the code base in place where it is starting to look like a scene with only the nessary code in it.</t>
   </si>
   <si>
-    <t>Get multiple rendered using Vulkan.</t>
-  </si>
-  <si>
     <t>Get a cube rendered using Vulkan.</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t>Got lighting implemented on the CPU side with it being threaded in order to make it run fast enough.</t>
   </si>
   <si>
-    <t>Got a basic LGH working with it apporximating the lights, although still is a bit dodgy when the particles are up close to the model.</t>
-  </si>
-  <si>
     <t>Look more into the LGH and how to implement better as well as getting the lighting on the GPU.</t>
   </si>
   <si>
@@ -182,6 +176,12 @@
   </si>
   <si>
     <t>Got lighting working on the GPU.</t>
+  </si>
+  <si>
+    <t>Get multiple cubes rendered using Vulkan.</t>
+  </si>
+  <si>
+    <t>Got a basic LGH working with it approximating the lights, although still is a bit dodgy when the particles are up close to the model.</t>
   </si>
 </sst>
 </file>
@@ -219,7 +219,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -252,21 +252,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -323,24 +308,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -363,47 +335,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -687,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,17 +669,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13">
+      <c r="A1" s="18">
         <v>17019105</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -724,11 +693,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="19">
         <v>43753</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>10</v>
@@ -738,11 +707,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="A4" s="5">
         <v>43760</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>11</v>
@@ -752,11 +721,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="A5" s="5">
         <v>43767</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>12</v>
@@ -766,11 +735,11 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="A6" s="5">
         <v>43774</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>13</v>
@@ -780,23 +749,25 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="A7" s="5">
         <v>43781</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="11" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="5">
         <v>43788</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>5</v>
@@ -806,11 +777,11 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="A9" s="5">
         <v>43795</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>4</v>
@@ -820,7 +791,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="A10" s="5">
         <v>43802</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -834,7 +805,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="A11" s="5">
         <v>43836</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -848,16 +819,16 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+      <c r="A12" s="20">
         <v>43842</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="15" t="s">
         <v>21</v>
       </c>
     </row>
@@ -865,7 +836,7 @@
       <c r="A13" s="5">
         <v>43849</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -879,14 +850,14 @@
       <c r="A14" s="5">
         <v>43856</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="11" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -894,13 +865,13 @@
         <v>43863</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -908,13 +879,13 @@
         <v>43870</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -922,13 +893,13 @@
         <v>43891</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="D17" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -936,13 +907,13 @@
         <v>43898</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -950,13 +921,13 @@
         <v>43905</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -964,177 +935,177 @@
         <v>43920</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="13"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="13"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
+      <c r="A23" s="13"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="A24" s="13"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="13"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+      <c r="A26" s="13"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="A27" s="13"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
+      <c r="A28" s="13"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
+      <c r="A29" s="13"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
+      <c r="A30" s="13"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
+      <c r="A31" s="13"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
+      <c r="A32" s="13"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+      <c r="A33" s="13"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
+      <c r="A34" s="13"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="13"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
+      <c r="A36" s="13"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
+      <c r="A37" s="13"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
+      <c r="A38" s="13"/>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
+      <c r="A39" s="13"/>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
+      <c r="A40" s="13"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
+      <c r="A41" s="13"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
+      <c r="A42" s="13"/>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
+      <c r="A43" s="13"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
+      <c r="A44" s="13"/>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
+      <c r="A45" s="13"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
+      <c r="A46" s="13"/>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
+      <c r="A47" s="13"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
+      <c r="A48" s="13"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
+      <c r="A49" s="13"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
+      <c r="A50" s="13"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
+      <c r="A51" s="13"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
+      <c r="A52" s="13"/>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
+      <c r="A53" s="13"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
+      <c r="A54" s="13"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
+      <c r="A55" s="13"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
+      <c r="A56" s="13"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
+      <c r="A57" s="13"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
+      <c r="A58" s="13"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
+      <c r="A59" s="13"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="16"/>
+      <c r="A60" s="13"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="16"/>
+      <c r="A61" s="13"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="16"/>
+      <c r="A62" s="13"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="16"/>
+      <c r="A63" s="13"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
+      <c r="A64" s="13"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="16"/>
+      <c r="A65" s="13"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="16"/>
+      <c r="A66" s="13"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="16"/>
+      <c r="A67" s="13"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="16"/>
+      <c r="A68" s="13"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="16"/>
+      <c r="A69" s="13"/>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="16"/>
+      <c r="A70" s="13"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="16"/>
+      <c r="A71" s="13"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="16"/>
+      <c r="A72" s="13"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="16"/>
+      <c r="A73" s="13"/>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="16"/>
+      <c r="A74" s="13"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="16"/>
+      <c r="A75" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>